<commit_message>
:sparkles: Added classification part.
</commit_message>
<xml_diff>
--- a/xueqiu_stock/stock_index_data/BJ899050.xlsx
+++ b/xueqiu_stock/stock_index_data/BJ899050.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P3"/>
+  <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -614,7 +614,6 @@
       <c r="I3" t="n">
         <v>1268900</v>
       </c>
-      <c r="J3" t="inlineStr"/>
       <c r="K3" t="n">
         <v>748.5</v>
       </c>
@@ -631,6 +630,66 @@
         <v>1079.71</v>
       </c>
       <c r="P3" t="n">
+        <v>702.55</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Tue Oct 31 00:50:03 2023</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>BJ899050</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>北证50</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>未开盘</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>760.89</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>+3.76  +0.50%</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
+        <v>760.89</v>
+      </c>
+      <c r="H4" t="n">
+        <v>751.45</v>
+      </c>
+      <c r="I4" t="n">
+        <v>1268900</v>
+      </c>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="n">
+        <v>748.5</v>
+      </c>
+      <c r="L4" t="n">
+        <v>757.13</v>
+      </c>
+      <c r="M4" t="n">
+        <v>1267000000</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0.016</v>
+      </c>
+      <c r="O4" t="n">
+        <v>1079.71</v>
+      </c>
+      <c r="P4" t="n">
         <v>702.55</v>
       </c>
     </row>

</xml_diff>